<commit_message>
Ajout de l'animation en spirale
</commit_message>
<xml_diff>
--- a/CodeArduino/Chiffres.xlsx
+++ b/CodeArduino/Chiffres.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171026"/>
   <extLst>
@@ -59,7 +60,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -147,11 +148,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -168,17 +258,38 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DP11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S2" workbookViewId="0">
+    <sheetView topLeftCell="S2" workbookViewId="0">
       <selection activeCell="B11" sqref="B11:AO11"/>
     </sheetView>
   </sheetViews>
@@ -1435,140 +1546,140 @@
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17">
+      <c r="B7" s="14"/>
+      <c r="C7" s="15">
         <v>0</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17">
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15">
         <v>48</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17">
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15">
         <v>49</v>
       </c>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="17">
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="15">
         <v>50</v>
       </c>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="17">
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="15">
         <v>51</v>
       </c>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="17">
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="15">
         <v>52</v>
       </c>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="17">
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="15">
         <v>53</v>
       </c>
-      <c r="AB7" s="17"/>
-      <c r="AC7" s="17"/>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="17">
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="15">
         <v>54</v>
       </c>
-      <c r="AF7" s="17"/>
-      <c r="AG7" s="17"/>
-      <c r="AH7" s="16"/>
-      <c r="AI7" s="17">
+      <c r="AF7" s="15"/>
+      <c r="AG7" s="15"/>
+      <c r="AH7" s="14"/>
+      <c r="AI7" s="15">
         <v>55</v>
       </c>
-      <c r="AJ7" s="17"/>
-      <c r="AK7" s="17"/>
-      <c r="AL7" s="16"/>
-      <c r="AM7" s="17">
+      <c r="AJ7" s="15"/>
+      <c r="AK7" s="15"/>
+      <c r="AL7" s="14"/>
+      <c r="AM7" s="15">
         <v>56</v>
       </c>
-      <c r="AN7" s="17"/>
-      <c r="AO7" s="17"/>
-      <c r="AP7" s="16"/>
-      <c r="AQ7" s="17">
+      <c r="AN7" s="15"/>
+      <c r="AO7" s="15"/>
+      <c r="AP7" s="14"/>
+      <c r="AQ7" s="15">
         <v>57</v>
       </c>
-      <c r="AR7" s="17"/>
-      <c r="AS7" s="17"/>
+      <c r="AR7" s="15"/>
+      <c r="AS7" s="15"/>
     </row>
     <row r="8" spans="1:120" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
-      <c r="C8" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
+      <c r="C8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="15">
+      <c r="G8" s="13">
         <v>0</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="15">
-        <v>1</v>
-      </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
+      <c r="K8" s="13">
+        <v>1</v>
+      </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
       <c r="N8" s="12"/>
-      <c r="O8" s="15">
+      <c r="O8" s="13">
         <v>2</v>
       </c>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
       <c r="R8" s="12"/>
-      <c r="S8" s="15">
+      <c r="S8" s="13">
         <v>3</v>
       </c>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
       <c r="V8" s="12"/>
-      <c r="W8" s="15">
+      <c r="W8" s="13">
         <v>4</v>
       </c>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
       <c r="Z8" s="12"/>
-      <c r="AA8" s="15">
+      <c r="AA8" s="13">
         <v>5</v>
       </c>
-      <c r="AB8" s="15"/>
-      <c r="AC8" s="15"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
       <c r="AD8" s="12"/>
-      <c r="AE8" s="15">
+      <c r="AE8" s="13">
         <v>6</v>
       </c>
-      <c r="AF8" s="15"/>
-      <c r="AG8" s="15"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
       <c r="AH8" s="12"/>
-      <c r="AI8" s="15">
+      <c r="AI8" s="13">
         <v>7</v>
       </c>
-      <c r="AJ8" s="15"/>
-      <c r="AK8" s="15"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
       <c r="AL8" s="12"/>
-      <c r="AM8" s="15">
+      <c r="AM8" s="13">
         <v>8</v>
       </c>
-      <c r="AN8" s="15"/>
-      <c r="AO8" s="15"/>
+      <c r="AN8" s="13"/>
+      <c r="AO8" s="13"/>
       <c r="AP8" s="12"/>
-      <c r="AQ8" s="15">
+      <c r="AQ8" s="13">
         <v>9</v>
       </c>
-      <c r="AR8" s="15"/>
-      <c r="AS8" s="15"/>
+      <c r="AR8" s="13"/>
+      <c r="AS8" s="13"/>
     </row>
     <row r="9" spans="1:120" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
@@ -1586,7 +1697,7 @@
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12" t="str">
-        <f t="shared" ref="G9:Q9" si="1">DEC2HEX(IF(G2=1,16,0)+IF(G3=1,8,0)+IF(G4=1,4,0)+IF(G5=1,2,0)+IF(G6=1,1,0),2)</f>
+        <f t="shared" ref="G9" si="1">DEC2HEX(IF(G2=1,16,0)+IF(G3=1,8,0)+IF(G4=1,4,0)+IF(G5=1,2,0)+IF(G6=1,1,0),2)</f>
         <v>1F</v>
       </c>
       <c r="H9" s="12" t="str">
@@ -1599,7 +1710,7 @@
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12" t="str">
-        <f t="shared" ref="K9:Q9" si="2">DEC2HEX(IF(K2=1,16,0)+IF(K3=1,8,0)+IF(K4=1,4,0)+IF(K5=1,2,0)+IF(K6=1,1,0),2)</f>
+        <f t="shared" ref="K9" si="2">DEC2HEX(IF(K2=1,16,0)+IF(K3=1,8,0)+IF(K4=1,4,0)+IF(K5=1,2,0)+IF(K6=1,1,0),2)</f>
         <v>00</v>
       </c>
       <c r="L9" s="12" t="str">
@@ -1612,7 +1723,7 @@
       </c>
       <c r="N9" s="12"/>
       <c r="O9" s="12" t="str">
-        <f t="shared" ref="O9:Q9" si="3">DEC2HEX(IF(O2=1,16,0)+IF(O3=1,8,0)+IF(O4=1,4,0)+IF(O5=1,2,0)+IF(O6=1,1,0),2)</f>
+        <f t="shared" ref="O9" si="3">DEC2HEX(IF(O2=1,16,0)+IF(O3=1,8,0)+IF(O4=1,4,0)+IF(O5=1,2,0)+IF(O6=1,1,0),2)</f>
         <v>17</v>
       </c>
       <c r="P9" s="12" t="str">
@@ -1651,7 +1762,7 @@
       </c>
       <c r="Z9" s="12"/>
       <c r="AA9" s="12" t="str">
-        <f t="shared" ref="AA9:AK9" si="6">DEC2HEX(IF(AA2=1,16,0)+IF(AA3=1,8,0)+IF(AA4=1,4,0)+IF(AA5=1,2,0)+IF(AA6=1,1,0),2)</f>
+        <f t="shared" ref="AA9" si="6">DEC2HEX(IF(AA2=1,16,0)+IF(AA3=1,8,0)+IF(AA4=1,4,0)+IF(AA5=1,2,0)+IF(AA6=1,1,0),2)</f>
         <v>1D</v>
       </c>
       <c r="AB9" s="12" t="str">
@@ -1664,7 +1775,7 @@
       </c>
       <c r="AD9" s="12"/>
       <c r="AE9" s="12" t="str">
-        <f t="shared" ref="AE9:AK9" si="7">DEC2HEX(IF(AE2=1,16,0)+IF(AE3=1,8,0)+IF(AE4=1,4,0)+IF(AE5=1,2,0)+IF(AE6=1,1,0),2)</f>
+        <f t="shared" ref="AE9" si="7">DEC2HEX(IF(AE2=1,16,0)+IF(AE3=1,8,0)+IF(AE4=1,4,0)+IF(AE5=1,2,0)+IF(AE6=1,1,0),2)</f>
         <v>1F</v>
       </c>
       <c r="AF9" s="12" t="str">
@@ -1677,7 +1788,7 @@
       </c>
       <c r="AH9" s="12"/>
       <c r="AI9" s="12" t="str">
-        <f t="shared" ref="AI9:AK9" si="8">DEC2HEX(IF(AI2=1,16,0)+IF(AI3=1,8,0)+IF(AI4=1,4,0)+IF(AI5=1,2,0)+IF(AI6=1,1,0),2)</f>
+        <f t="shared" ref="AI9" si="8">DEC2HEX(IF(AI2=1,16,0)+IF(AI3=1,8,0)+IF(AI4=1,4,0)+IF(AI5=1,2,0)+IF(AI6=1,1,0),2)</f>
         <v>10</v>
       </c>
       <c r="AJ9" s="12" t="str">
@@ -1716,108 +1827,108 @@
       </c>
     </row>
     <row r="10" spans="1:120" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="str">
+      <c r="B10" s="16" t="str">
         <f>_xlfn.CONCAT("0x",C9,",0x",D9,",0x",E9,",//",C7,"--&gt;",C8,"
 ")</f>
         <v xml:space="preserve">0x00,0x00,0x00,//0--&gt;" "
 </v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13" t="str">
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16" t="str">
         <f t="shared" ref="F10" si="11">_xlfn.CONCAT("0x",G9,",0x",H9,",0x",I9,",//",G7,"--&gt;",G8,"
 ")</f>
         <v xml:space="preserve">0x1F,0x11,0x1F,//48--&gt;0
 </v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13" t="str">
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16" t="str">
         <f t="shared" ref="J10" si="12">_xlfn.CONCAT("0x",K9,",0x",L9,",0x",M9,",//",K7,"--&gt;",K8,"
 ")</f>
         <v xml:space="preserve">0x00,0x1F,0x00,//49--&gt;1
 </v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13" t="str">
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16" t="str">
         <f t="shared" ref="N10" si="13">_xlfn.CONCAT("0x",O9,",0x",P9,",0x",Q9,",//",O7,"--&gt;",O8,"
 ")</f>
         <v xml:space="preserve">0x17,0x15,0x1D,//50--&gt;2
 </v>
       </c>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13" t="str">
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16" t="str">
         <f t="shared" ref="R10" si="14">_xlfn.CONCAT("0x",S9,",0x",T9,",0x",U9,",//",S7,"--&gt;",S8,"
 ")</f>
         <v xml:space="preserve">0x11,0x15,0x1F,//51--&gt;3
 </v>
       </c>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13" t="str">
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16" t="str">
         <f t="shared" ref="V10" si="15">_xlfn.CONCAT("0x",W9,",0x",X9,",0x",Y9,",//",W7,"--&gt;",W8,"
 ")</f>
         <v xml:space="preserve">0x1E,0x02,0x07,//52--&gt;4
 </v>
       </c>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13" t="str">
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16" t="str">
         <f t="shared" ref="Z10" si="16">_xlfn.CONCAT("0x",AA9,",0x",AB9,",0x",AC9,",//",AA7,"--&gt;",AA8,"
 ")</f>
         <v xml:space="preserve">0x1D,0x15,0x17,//53--&gt;5
 </v>
       </c>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13" t="str">
+      <c r="AA10" s="16"/>
+      <c r="AB10" s="16"/>
+      <c r="AC10" s="16"/>
+      <c r="AD10" s="16" t="str">
         <f t="shared" ref="AD10" si="17">_xlfn.CONCAT("0x",AE9,",0x",AF9,",0x",AG9,",//",AE7,"--&gt;",AE8,"
 ")</f>
         <v xml:space="preserve">0x1F,0x15,0x07,//54--&gt;6
 </v>
       </c>
-      <c r="AE10" s="13"/>
-      <c r="AF10" s="13"/>
-      <c r="AG10" s="13"/>
-      <c r="AH10" s="13" t="str">
+      <c r="AE10" s="16"/>
+      <c r="AF10" s="16"/>
+      <c r="AG10" s="16"/>
+      <c r="AH10" s="16" t="str">
         <f t="shared" ref="AH10" si="18">_xlfn.CONCAT("0x",AI9,",0x",AJ9,",0x",AK9,",//",AI7,"--&gt;",AI8,"
 ")</f>
         <v xml:space="preserve">0x10,0x10,0x1F,//55--&gt;7
 </v>
       </c>
-      <c r="AI10" s="13"/>
-      <c r="AJ10" s="13"/>
-      <c r="AK10" s="13"/>
-      <c r="AL10" s="13" t="str">
+      <c r="AI10" s="16"/>
+      <c r="AJ10" s="16"/>
+      <c r="AK10" s="16"/>
+      <c r="AL10" s="16" t="str">
         <f t="shared" ref="AL10" si="19">_xlfn.CONCAT("0x",AM9,",0x",AN9,",0x",AO9,",//",AM7,"--&gt;",AM8,"
 ")</f>
         <v xml:space="preserve">0x1F,0x15,0x1F,//56--&gt;8
 </v>
       </c>
-      <c r="AM10" s="13"/>
-      <c r="AN10" s="13"/>
-      <c r="AO10" s="13"/>
-      <c r="AP10" s="13" t="str">
+      <c r="AM10" s="16"/>
+      <c r="AN10" s="16"/>
+      <c r="AO10" s="16"/>
+      <c r="AP10" s="16" t="str">
         <f t="shared" ref="AP10" si="20">_xlfn.CONCAT("0x",AQ9,",0x",AR9,",0x",AS9,",//",AQ7,"--&gt;",AQ8,"
 ")</f>
         <v xml:space="preserve">0x1C,0x15,0x1F,//57--&gt;9
 </v>
       </c>
-      <c r="AQ10" s="13"/>
-      <c r="AR10" s="13"/>
-      <c r="AS10" s="13"/>
+      <c r="AQ10" s="16"/>
+      <c r="AR10" s="16"/>
+      <c r="AS10" s="16"/>
     </row>
     <row r="11" spans="1:120" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="str">
+      <c r="B11" s="17" t="str">
         <f>_xlfn.CONCAT(B10:AS10)</f>
         <v xml:space="preserve">0x00,0x00,0x00,//0--&gt;" "
 0x1F,0x11,0x1F,//48--&gt;0
@@ -1832,53 +1943,48 @@
 0x1C,0x15,0x1F,//57--&gt;9
 </v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="14"/>
-      <c r="AG11" s="14"/>
-      <c r="AH11" s="14"/>
-      <c r="AI11" s="14"/>
-      <c r="AJ11" s="14"/>
-      <c r="AK11" s="14"/>
-      <c r="AL11" s="14"/>
-      <c r="AM11" s="14"/>
-      <c r="AN11" s="14"/>
-      <c r="AO11" s="14"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17"/>
+      <c r="AG11" s="17"/>
+      <c r="AH11" s="17"/>
+      <c r="AI11" s="17"/>
+      <c r="AJ11" s="17"/>
+      <c r="AK11" s="17"/>
+      <c r="AL11" s="17"/>
+      <c r="AM11" s="17"/>
+      <c r="AN11" s="17"/>
+      <c r="AO11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="Z10:AC10"/>
-    <mergeCell ref="AD10:AG10"/>
-    <mergeCell ref="AH10:AK10"/>
-    <mergeCell ref="AL10:AO10"/>
-    <mergeCell ref="AP10:AS10"/>
     <mergeCell ref="B11:AO11"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="F10:I10"/>
@@ -1886,6 +1992,11 @@
     <mergeCell ref="N10:Q10"/>
     <mergeCell ref="R10:U10"/>
     <mergeCell ref="V10:Y10"/>
+    <mergeCell ref="Z10:AC10"/>
+    <mergeCell ref="AD10:AG10"/>
+    <mergeCell ref="AH10:AK10"/>
+    <mergeCell ref="AL10:AO10"/>
+    <mergeCell ref="AP10:AS10"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD6">
     <cfRule type="colorScale" priority="1">
@@ -1900,4 +2011,514 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="4.28515625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22">
+        <v>2</v>
+      </c>
+      <c r="D1" s="22">
+        <v>3</v>
+      </c>
+      <c r="E1" s="22">
+        <v>4</v>
+      </c>
+      <c r="F1" s="22">
+        <v>5</v>
+      </c>
+      <c r="G1" s="22">
+        <v>6</v>
+      </c>
+      <c r="H1" s="22">
+        <v>7</v>
+      </c>
+      <c r="I1" s="22">
+        <v>8</v>
+      </c>
+      <c r="J1" s="22">
+        <v>9</v>
+      </c>
+      <c r="K1" s="22">
+        <v>10</v>
+      </c>
+      <c r="L1" s="23">
+        <v>11</v>
+      </c>
+      <c r="M1" s="18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19">
+        <v>25</v>
+      </c>
+      <c r="B2" s="18">
+        <v>24</v>
+      </c>
+      <c r="C2" s="21">
+        <v>23</v>
+      </c>
+      <c r="D2" s="22">
+        <v>22</v>
+      </c>
+      <c r="E2" s="22">
+        <v>21</v>
+      </c>
+      <c r="F2" s="22">
+        <v>20</v>
+      </c>
+      <c r="G2" s="22">
+        <v>19</v>
+      </c>
+      <c r="H2" s="22">
+        <v>18</v>
+      </c>
+      <c r="I2" s="22">
+        <v>17</v>
+      </c>
+      <c r="J2" s="22">
+        <v>16</v>
+      </c>
+      <c r="K2" s="23">
+        <v>15</v>
+      </c>
+      <c r="L2" s="18">
+        <v>14</v>
+      </c>
+      <c r="M2" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19">
+        <v>26</v>
+      </c>
+      <c r="B3" s="19">
+        <v>27</v>
+      </c>
+      <c r="C3" s="18">
+        <v>28</v>
+      </c>
+      <c r="D3" s="21">
+        <v>29</v>
+      </c>
+      <c r="E3" s="22">
+        <v>30</v>
+      </c>
+      <c r="F3" s="22">
+        <v>31</v>
+      </c>
+      <c r="G3" s="22">
+        <v>32</v>
+      </c>
+      <c r="H3" s="22">
+        <v>33</v>
+      </c>
+      <c r="I3" s="22">
+        <v>34</v>
+      </c>
+      <c r="J3" s="23">
+        <v>35</v>
+      </c>
+      <c r="K3" s="18">
+        <v>36</v>
+      </c>
+      <c r="L3" s="19">
+        <v>37</v>
+      </c>
+      <c r="M3" s="19">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <v>51</v>
+      </c>
+      <c r="B4" s="19">
+        <v>50</v>
+      </c>
+      <c r="C4" s="19">
+        <v>49</v>
+      </c>
+      <c r="D4" s="18">
+        <v>48</v>
+      </c>
+      <c r="E4" s="21">
+        <v>47</v>
+      </c>
+      <c r="F4" s="22">
+        <v>46</v>
+      </c>
+      <c r="G4" s="22">
+        <v>45</v>
+      </c>
+      <c r="H4" s="22">
+        <v>44</v>
+      </c>
+      <c r="I4" s="23">
+        <v>43</v>
+      </c>
+      <c r="J4" s="18">
+        <v>42</v>
+      </c>
+      <c r="K4" s="19">
+        <v>41</v>
+      </c>
+      <c r="L4" s="19">
+        <v>40</v>
+      </c>
+      <c r="M4" s="19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19">
+        <v>52</v>
+      </c>
+      <c r="B5" s="19">
+        <v>53</v>
+      </c>
+      <c r="C5" s="19">
+        <v>54</v>
+      </c>
+      <c r="D5" s="19">
+        <v>55</v>
+      </c>
+      <c r="E5" s="18">
+        <v>56</v>
+      </c>
+      <c r="F5" s="21">
+        <v>57</v>
+      </c>
+      <c r="G5" s="22">
+        <v>58</v>
+      </c>
+      <c r="H5" s="23">
+        <v>59</v>
+      </c>
+      <c r="I5" s="18">
+        <v>60</v>
+      </c>
+      <c r="J5" s="19">
+        <v>61</v>
+      </c>
+      <c r="K5" s="19">
+        <v>62</v>
+      </c>
+      <c r="L5" s="19">
+        <v>63</v>
+      </c>
+      <c r="M5" s="19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>77</v>
+      </c>
+      <c r="B6" s="19">
+        <v>76</v>
+      </c>
+      <c r="C6" s="19">
+        <v>75</v>
+      </c>
+      <c r="D6" s="19">
+        <v>74</v>
+      </c>
+      <c r="E6" s="19">
+        <v>73</v>
+      </c>
+      <c r="F6" s="24">
+        <v>72</v>
+      </c>
+      <c r="G6" s="24">
+        <v>71</v>
+      </c>
+      <c r="H6" s="18">
+        <v>70</v>
+      </c>
+      <c r="I6" s="19">
+        <v>69</v>
+      </c>
+      <c r="J6" s="19">
+        <v>68</v>
+      </c>
+      <c r="K6" s="19">
+        <v>67</v>
+      </c>
+      <c r="L6" s="19">
+        <v>66</v>
+      </c>
+      <c r="M6" s="19">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
+        <v>78</v>
+      </c>
+      <c r="B7" s="19">
+        <v>79</v>
+      </c>
+      <c r="C7" s="19">
+        <v>80</v>
+      </c>
+      <c r="D7" s="19">
+        <v>81</v>
+      </c>
+      <c r="E7" s="20">
+        <v>82</v>
+      </c>
+      <c r="F7" s="21">
+        <v>83</v>
+      </c>
+      <c r="G7" s="23">
+        <v>84</v>
+      </c>
+      <c r="H7" s="20">
+        <v>85</v>
+      </c>
+      <c r="I7" s="19">
+        <v>86</v>
+      </c>
+      <c r="J7" s="19">
+        <v>87</v>
+      </c>
+      <c r="K7" s="19">
+        <v>88</v>
+      </c>
+      <c r="L7" s="19">
+        <v>89</v>
+      </c>
+      <c r="M7" s="19">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>103</v>
+      </c>
+      <c r="B8" s="19">
+        <v>102</v>
+      </c>
+      <c r="C8" s="19">
+        <v>101</v>
+      </c>
+      <c r="D8" s="20">
+        <v>100</v>
+      </c>
+      <c r="E8" s="21">
+        <v>99</v>
+      </c>
+      <c r="F8" s="22">
+        <v>98</v>
+      </c>
+      <c r="G8" s="22">
+        <v>97</v>
+      </c>
+      <c r="H8" s="23">
+        <v>96</v>
+      </c>
+      <c r="I8" s="20">
+        <v>95</v>
+      </c>
+      <c r="J8" s="19">
+        <v>94</v>
+      </c>
+      <c r="K8" s="19">
+        <v>93</v>
+      </c>
+      <c r="L8" s="19">
+        <v>92</v>
+      </c>
+      <c r="M8" s="19">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
+        <v>104</v>
+      </c>
+      <c r="B9" s="19">
+        <v>105</v>
+      </c>
+      <c r="C9" s="20">
+        <v>106</v>
+      </c>
+      <c r="D9" s="21">
+        <v>107</v>
+      </c>
+      <c r="E9" s="22">
+        <v>108</v>
+      </c>
+      <c r="F9" s="22">
+        <v>109</v>
+      </c>
+      <c r="G9" s="22">
+        <v>110</v>
+      </c>
+      <c r="H9" s="22">
+        <v>111</v>
+      </c>
+      <c r="I9" s="23">
+        <v>112</v>
+      </c>
+      <c r="J9" s="20">
+        <v>113</v>
+      </c>
+      <c r="K9" s="19">
+        <v>114</v>
+      </c>
+      <c r="L9" s="19">
+        <v>115</v>
+      </c>
+      <c r="M9" s="19">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <v>129</v>
+      </c>
+      <c r="B10" s="20">
+        <v>128</v>
+      </c>
+      <c r="C10" s="21">
+        <v>127</v>
+      </c>
+      <c r="D10" s="22">
+        <v>126</v>
+      </c>
+      <c r="E10" s="22">
+        <v>125</v>
+      </c>
+      <c r="F10" s="22">
+        <v>124</v>
+      </c>
+      <c r="G10" s="22">
+        <v>123</v>
+      </c>
+      <c r="H10" s="22">
+        <v>122</v>
+      </c>
+      <c r="I10" s="22">
+        <v>121</v>
+      </c>
+      <c r="J10" s="23">
+        <v>120</v>
+      </c>
+      <c r="K10" s="20">
+        <v>119</v>
+      </c>
+      <c r="L10" s="19">
+        <v>118</v>
+      </c>
+      <c r="M10" s="19">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>130</v>
+      </c>
+      <c r="B11" s="21">
+        <v>131</v>
+      </c>
+      <c r="C11" s="22">
+        <v>132</v>
+      </c>
+      <c r="D11" s="22">
+        <v>133</v>
+      </c>
+      <c r="E11" s="22">
+        <v>134</v>
+      </c>
+      <c r="F11" s="22">
+        <v>135</v>
+      </c>
+      <c r="G11" s="22">
+        <v>136</v>
+      </c>
+      <c r="H11" s="22">
+        <v>137</v>
+      </c>
+      <c r="I11" s="22">
+        <v>138</v>
+      </c>
+      <c r="J11" s="22">
+        <v>139</v>
+      </c>
+      <c r="K11" s="23">
+        <v>140</v>
+      </c>
+      <c r="L11" s="20">
+        <v>141</v>
+      </c>
+      <c r="M11" s="19">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>155</v>
+      </c>
+      <c r="B12" s="22">
+        <v>154</v>
+      </c>
+      <c r="C12" s="22">
+        <v>153</v>
+      </c>
+      <c r="D12" s="22">
+        <v>152</v>
+      </c>
+      <c r="E12" s="22">
+        <v>151</v>
+      </c>
+      <c r="F12" s="22">
+        <v>150</v>
+      </c>
+      <c r="G12" s="22">
+        <v>149</v>
+      </c>
+      <c r="H12" s="22">
+        <v>148</v>
+      </c>
+      <c r="I12" s="22">
+        <v>147</v>
+      </c>
+      <c r="J12" s="22">
+        <v>146</v>
+      </c>
+      <c r="K12" s="22">
+        <v>145</v>
+      </c>
+      <c r="L12" s="23">
+        <v>144</v>
+      </c>
+      <c r="M12" s="20">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>